<commit_message>
Added classes for text processing.
</commit_message>
<xml_diff>
--- a/server/data/data.xlsx
+++ b/server/data/data.xlsx
@@ -20,21 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
-  <si>
-    <t>Пахота зяби под мн тр
-По Пу 26/488
-Отд 12 26/221
-Предп культ под оз пш
-По Пу 215/1015
-Отд 12 128/317
-Отд 16 123/529
-2-е диск сах св под пш
-По Пу 22/627
-Отд 11 22/217
-2-е диск сои под оз пш
-По Пу 45/1907
-Отд 12 45/299</t>
-  </si>
   <si>
     <t>Пахота зяби под мн тр
 По Пу 26/514
@@ -1362,6 +1347,21 @@
 Отд 11-102/209
 Отд 12-175/593
 Отд 17-177/260</t>
+  </si>
+  <si>
+    <t>Похота зяби под мн тр
+По Пу 26/488
+Отд 12 26/221
+Предп культ под оз пш
+По Пу 215/1015
+Отд 12 128/317
+Отд 16 123/529
+2-е диск сах св под пш
+По Пу 22/627
+Отд 11 22/217
+2-е диск сои под оз пш
+По Пу 45/1907
+Отд 12 45/299</t>
   </si>
 </sst>
 </file>
@@ -1715,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A106"/>
+  <dimension ref="A2:A107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,249 +1726,244 @@
     <col min="1" max="1" width="63.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:1" ht="240" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="345" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="345" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:1" ht="345" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="345" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="225" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="285" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="285" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="270" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="270" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="240" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="28" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="360" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="360" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="43" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="405" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" ht="405" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="345" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="345" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="47" spans="1:1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="90" x14ac:dyDescent="0.25">
@@ -1976,107 +1971,107 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="56" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="59" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="61" spans="1:1" ht="285" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="285" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="63" spans="1:1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="270" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="65" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:1" ht="240" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -2086,54 +2081,54 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="78" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="79" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="80" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="195" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2143,50 +2138,50 @@
     </row>
     <row r="84" spans="1:1" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="87" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="330" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="330" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>79</v>
       </c>
@@ -2196,64 +2191,69 @@
         <v>78</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="285" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="285" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="165" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="210" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to fix spell checker. Unsuccessfully.
</commit_message>
<xml_diff>
--- a/server/data/data.xlsx
+++ b/server/data/data.xlsx
@@ -1349,7 +1349,7 @@
 Отд 17-177/260</t>
   </si>
   <si>
-    <t>Похота зяби под мн тр
+    <t>Пахота зяби под мн тр
 По Пу 26/488
 Отд 12 26/221
 Предп культ под оз пш
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>